<commit_message>
Make from and report Subcommittee
</commit_message>
<xml_diff>
--- a/Report_EGAT.xlsx
+++ b/Report_EGAT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\this\Documents\GitHub\Pa_DevEgatlums\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\this\Documents\GitHub\Pa_DevEgat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="24000" windowHeight="9585" tabRatio="844"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="24000" windowHeight="9585" tabRatio="844"/>
   </bookViews>
   <sheets>
     <sheet name="1. ระบบสมาชิก | อนุกรรมการ" sheetId="2" r:id="rId1"/>
@@ -849,12 +849,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -864,6 +858,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,34 +1197,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
@@ -1233,8 +1233,8 @@
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
@@ -1413,28 +1413,28 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="23">
+    <row r="19" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21">
         <v>9</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26" t="s">
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="I19" s="25" t="s">
+      <c r="I19" s="23" t="s">
         <v>212</v>
       </c>
     </row>
@@ -1807,34 +1807,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
@@ -1843,8 +1843,8 @@
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
@@ -2319,34 +2319,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="18"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2374,11 +2374,11 @@
       <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="19"/>
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -2925,11 +2925,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="18"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -2937,59 +2937,59 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="19"/>
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -3536,51 +3536,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="18"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="2"/>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="26"/>
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
@@ -4112,25 +4112,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4142,35 +4142,35 @@
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="19"/>
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4644,83 +4644,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="19"/>
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Create CommitteeAppoint And CommitteeCancel
</commit_message>
<xml_diff>
--- a/Report_EGAT.xlsx
+++ b/Report_EGAT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="24000" windowHeight="9585" tabRatio="844"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="24000" windowHeight="9585" tabRatio="844"/>
   </bookViews>
   <sheets>
     <sheet name="1. ระบบสมาชิก | อนุกรรมการ" sheetId="2" r:id="rId1"/>
@@ -323,9 +323,6 @@
     <t>รายงานสมัครใหม่ (อนุกรรมการ สร.กฟผ.)</t>
   </si>
   <si>
-    <t>รายงานยกเลิก (อนุกรรมการ สร.กฟผ.)</t>
-  </si>
-  <si>
     <t xml:space="preserve">รายงานคำสั่งแต่งตั้งอนุกรรมการ </t>
   </si>
   <si>
@@ -723,13 +720,28 @@
   </si>
   <si>
     <t>Sitthipong</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">รายงานยกเลิก (อนุกรรมการ สร.กฟผ.) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*รายงานการสิ้นสภาพ (อนุกรรมการ สร.กฟผ.)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,6 +761,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1181,14 +1200,14 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="62.625" customWidth="1"/>
+    <col min="3" max="3" width="66.25" customWidth="1"/>
     <col min="4" max="4" width="51.125" customWidth="1"/>
     <col min="5" max="5" width="29.125" customWidth="1"/>
     <col min="6" max="6" width="58.875" customWidth="1"/>
@@ -1247,22 +1266,22 @@
         <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>201</v>
-      </c>
       <c r="H12" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1270,13 +1289,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>94</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1284,10 +1303,10 @@
         <v>93</v>
       </c>
       <c r="H13" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1295,23 +1314,23 @@
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
         <v>93</v>
       </c>
       <c r="H14" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1319,26 +1338,26 @@
         <v>3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>93</v>
       </c>
       <c r="H15" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1346,25 +1365,25 @@
         <v>4</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>93</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1372,22 +1391,22 @@
         <v>5</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1395,22 +1414,22 @@
         <v>6</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
@@ -1418,13 +1437,13 @@
         <v>9</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -1432,60 +1451,60 @@
         <v>93</v>
       </c>
       <c r="H19" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21">
+        <v>10</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="I19" s="23" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>10</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="21">
+        <v>11</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>11</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>212</v>
+      <c r="H21" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1493,26 +1512,26 @@
         <v>12</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>93</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1520,26 +1539,26 @@
         <v>13</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1547,22 +1566,22 @@
         <v>14</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1570,22 +1589,22 @@
         <v>15</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1784,6 +1803,7 @@
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1857,22 +1877,22 @@
         <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>201</v>
-      </c>
       <c r="H12" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1880,13 +1900,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1899,17 +1919,17 @@
         <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -1919,10 +1939,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="6"/>
@@ -1936,10 +1956,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="20"/>
       <c r="F16" s="6"/>
@@ -1952,10 +1972,10 @@
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1969,10 +1989,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1986,10 +2006,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -2003,10 +2023,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -2020,10 +2040,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -2037,10 +2057,10 @@
         <v>10</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -2054,10 +2074,10 @@
         <v>11</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="3"/>
@@ -2071,10 +2091,10 @@
         <v>12</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -2088,10 +2108,10 @@
         <v>13</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="6"/>
@@ -2392,22 +2412,22 @@
         <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>201</v>
-      </c>
       <c r="H12" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2418,13 +2438,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -2437,13 +2457,13 @@
         <v>3</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -2456,7 +2476,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -2473,13 +2493,13 @@
         <v>3</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -2492,7 +2512,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -2506,16 +2526,16 @@
         <v>6</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -2525,15 +2545,15 @@
         <v>7</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -2544,15 +2564,15 @@
         <v>8</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -2563,10 +2583,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -2580,10 +2600,10 @@
         <v>10</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -2597,10 +2617,10 @@
         <v>11</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -2614,10 +2634,10 @@
         <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -2631,10 +2651,10 @@
         <v>13</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -2648,16 +2668,16 @@
         <v>14</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -2667,15 +2687,15 @@
         <v>15</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -2686,15 +2706,15 @@
         <v>16</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -2705,10 +2725,10 @@
         <v>17</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -2722,10 +2742,10 @@
         <v>18</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -2739,10 +2759,10 @@
         <v>19</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -2756,16 +2776,16 @@
         <v>20</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -2775,15 +2795,15 @@
         <v>21</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -2794,10 +2814,10 @@
         <v>22</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -3003,22 +3023,22 @@
         <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>201</v>
-      </c>
       <c r="H12" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -3029,11 +3049,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -3048,11 +3068,11 @@
         <v>8</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D14" s="20"/>
       <c r="F14" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -3066,7 +3086,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -3083,12 +3103,12 @@
         <v>10</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D16" s="20"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -3101,15 +3121,15 @@
         <v>11</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -3122,7 +3142,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -3139,7 +3159,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -3156,7 +3176,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -3173,15 +3193,15 @@
         <v>13</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -3194,7 +3214,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="6"/>
@@ -3211,7 +3231,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="3"/>
@@ -3228,7 +3248,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -3245,7 +3265,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -3262,7 +3282,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -3279,7 +3299,7 @@
         <v>17</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -3296,7 +3316,7 @@
         <v>17</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -3313,7 +3333,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -3330,7 +3350,7 @@
         <v>17</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -3347,13 +3367,13 @@
         <v>17</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -3366,7 +3386,7 @@
         <v>17</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -3383,12 +3403,12 @@
         <v>17</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -3402,12 +3422,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D34" s="20"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3593,22 +3613,22 @@
         <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>201</v>
-      </c>
       <c r="H12" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -3980,7 +4000,7 @@
         <v>57</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -4121,13 +4141,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -4135,7 +4155,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -4143,7 +4163,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
@@ -4151,7 +4171,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -4159,7 +4179,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -4167,7 +4187,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -4184,22 +4204,22 @@
         <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>201</v>
-      </c>
       <c r="H12" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -4653,7 +4673,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -4661,7 +4681,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -4669,7 +4689,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
@@ -4677,7 +4697,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
@@ -4685,7 +4705,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -4693,7 +4713,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -4701,7 +4721,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -4709,7 +4729,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -4717,7 +4737,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -4734,22 +4754,22 @@
         <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>201</v>
-      </c>
       <c r="H12" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>